<commit_message>
updates for MGIS in the table
</commit_message>
<xml_diff>
--- a/content/images/BrAPI_Application_Chart.xlsx
+++ b/content/images/BrAPI_Application_Chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps664\Documents\Letters_Reports_Publications\BrAPI-Manuscript2\content\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DD27B0-CA2C-4721-AE40-13E21416BDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3187F81-07ED-476D-AA40-49909491565A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8D6FC713-DE86-495E-930B-D50DF992A6EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D6FC713-DE86-495E-930B-D50DF992A6EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="38">
   <si>
     <t>Core</t>
   </si>
@@ -890,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:AB48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.2"/>
@@ -1467,7 +1467,9 @@
       <c r="B21" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="D21" s="26" t="s">
         <v>35</v>
       </c>
@@ -1477,7 +1479,9 @@
       <c r="H21" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I21" s="27"/>
+      <c r="I21" s="27" t="s">
+        <v>35</v>
+      </c>
       <c r="J21" s="27"/>
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>

</xml_diff>